<commit_message>
updated fig1, fig2, fig3 and part of fig4
</commit_message>
<xml_diff>
--- a/Fig_1/countermydata.xlsx
+++ b/Fig_1/countermydata.xlsx
@@ -1,40 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leona\Desktop\QoE_comsnet\QoE_combination\Fig_1\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE82161-A347-4C48-8B1D-B48EA3B4B65B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,21 +78,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -149,7 +122,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -183,7 +156,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -218,10 +190,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -394,40 +365,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B101"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B102" sqref="B102"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1">
         <v>1</v>
       </c>
       <c r="B1">
-        <v>0.59027777777777779</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.5902777777777778</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" s="1">
         <v>2</v>
       </c>
       <c r="B2">
-        <v>0.11805555555555559</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.1180555555555556</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="1">
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0.15277777777777779</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.1527777777777778</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="1">
         <v>4</v>
       </c>
@@ -435,15 +404,15 @@
         <v>0.2013888888888889</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="1">
         <v>5</v>
       </c>
       <c r="B5">
-        <v>0.25694444444444448</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.2569444444444445</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" s="1">
         <v>6</v>
       </c>
@@ -451,7 +420,7 @@
         <v>0.2986111111111111</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" s="1">
         <v>7</v>
       </c>
@@ -459,47 +428,47 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" s="1">
         <v>8</v>
       </c>
       <c r="B8">
-        <v>0.35416666666666657</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.3541666666666666</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" s="1">
         <v>9</v>
       </c>
       <c r="B9">
-        <v>0.29166666666666669</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.2916666666666667</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" s="1">
         <v>10</v>
       </c>
       <c r="B10">
-        <v>0.92361111111111116</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.9236111111111112</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11" s="1">
         <v>11</v>
       </c>
       <c r="B11">
-        <v>0.33333333333333343</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.3333333333333334</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" s="1">
         <v>12</v>
       </c>
       <c r="B12">
-        <v>0.34027777777777768</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.3402777777777777</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13" s="1">
         <v>13</v>
       </c>
@@ -507,31 +476,31 @@
         <v>0.3263888888888889</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2">
       <c r="A14" s="1">
         <v>14</v>
       </c>
       <c r="B14">
-        <v>0.34027777777777768</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.3402777777777777</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15" s="1">
         <v>15</v>
       </c>
       <c r="B15">
-        <v>0.54166666666666674</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.5416666666666667</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
       <c r="A16" s="1">
         <v>16</v>
       </c>
       <c r="B16">
-        <v>0.43055555555555558</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.4305555555555556</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" s="1">
         <v>17</v>
       </c>
@@ -539,63 +508,63 @@
         <v>0.3888888888888889</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" s="1">
         <v>18</v>
       </c>
       <c r="B18">
-        <v>0.40972222222222232</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.4097222222222223</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" s="1">
         <v>19</v>
       </c>
       <c r="B19">
-        <v>0.47222222222222221</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.4722222222222222</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" s="1">
         <v>20</v>
       </c>
       <c r="B20">
-        <v>1.4027777777777779</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1.402777777777778</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" s="1">
         <v>21</v>
       </c>
       <c r="B21">
-        <v>0.93055555555555547</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.9305555555555555</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" s="1">
         <v>22</v>
       </c>
       <c r="B22">
-        <v>0.79166666666666674</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.7916666666666667</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" s="1">
         <v>23</v>
       </c>
       <c r="B23">
-        <v>0.58333333333333337</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.5833333333333334</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" s="1">
         <v>24</v>
       </c>
       <c r="B24">
-        <v>0.63888888888888895</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.638888888888889</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25" s="1">
         <v>25</v>
       </c>
@@ -603,23 +572,23 @@
         <v>1.229166666666667</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2">
       <c r="A26" s="1">
         <v>26</v>
       </c>
       <c r="B26">
-        <v>0.54861111111111105</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.548611111111111</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
       <c r="A27" s="1">
         <v>27</v>
       </c>
       <c r="B27">
-        <v>0.53472222222222221</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.5347222222222222</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
       <c r="A28" s="1">
         <v>28</v>
       </c>
@@ -627,23 +596,23 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2">
       <c r="A29" s="1">
         <v>29</v>
       </c>
       <c r="B29">
-        <v>0.59722222222222221</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.5972222222222222</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30" s="1">
         <v>30</v>
       </c>
       <c r="B30">
-        <v>1.4722222222222221</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1.472222222222222</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31" s="1">
         <v>31</v>
       </c>
@@ -651,31 +620,31 @@
         <v>0.5625</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2">
       <c r="A32" s="1">
         <v>32</v>
       </c>
       <c r="B32">
-        <v>0.72222222222222221</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.7222222222222222</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
       <c r="A33" s="1">
         <v>33</v>
       </c>
       <c r="B33">
-        <v>0.72916666666666663</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.7291666666666666</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
       <c r="A34" s="1">
         <v>34</v>
       </c>
       <c r="B34">
-        <v>0.69444444444444442</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.6944444444444444</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
       <c r="A35" s="1">
         <v>35</v>
       </c>
@@ -683,23 +652,23 @@
         <v>1.180555555555556</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2">
       <c r="A36" s="1">
         <v>36</v>
       </c>
       <c r="B36">
-        <v>0.76388888888888884</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.7638888888888888</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
       <c r="A37" s="1">
         <v>37</v>
       </c>
       <c r="B37">
-        <v>0.65277777777777779</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.6527777777777778</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
       <c r="A38" s="1">
         <v>38</v>
       </c>
@@ -707,15 +676,15 @@
         <v>1.125</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2">
       <c r="A39" s="1">
         <v>39</v>
       </c>
       <c r="B39">
-        <v>0.90277777777777768</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.9027777777777777</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
       <c r="A40" s="1">
         <v>40</v>
       </c>
@@ -723,31 +692,31 @@
         <v>2.416666666666667</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2">
       <c r="A41" s="1">
         <v>41</v>
       </c>
       <c r="B41">
-        <v>1.5486111111111109</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1.548611111111111</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
       <c r="A42" s="1">
         <v>42</v>
       </c>
       <c r="B42">
-        <v>0.96527777777777779</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.9652777777777778</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
       <c r="A43" s="1">
         <v>43</v>
       </c>
       <c r="B43">
-        <v>0.97916666666666674</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.9791666666666667</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
       <c r="A44" s="1">
         <v>44</v>
       </c>
@@ -755,15 +724,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2">
       <c r="A45" s="1">
         <v>45</v>
       </c>
       <c r="B45">
-        <v>1.2638888888888891</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1.263888888888889</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
       <c r="A46" s="1">
         <v>46</v>
       </c>
@@ -771,23 +740,23 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2">
       <c r="A47" s="1">
         <v>47</v>
       </c>
       <c r="B47">
-        <v>0.59027777777777779</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.5902777777777778</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
       <c r="A48" s="1">
         <v>48</v>
       </c>
       <c r="B48">
-        <v>0.42361111111111122</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.4236111111111112</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
       <c r="A49" s="1">
         <v>49</v>
       </c>
@@ -795,15 +764,15 @@
         <v>0.2638888888888889</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2">
       <c r="A50" s="1">
         <v>50</v>
       </c>
       <c r="B50">
-        <v>5.4930555555555562</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5.493055555555556</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
       <c r="A51" s="1">
         <v>51</v>
       </c>
@@ -811,31 +780,31 @@
         <v>0.2986111111111111</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2">
       <c r="A52" s="1">
         <v>52</v>
       </c>
       <c r="B52">
-        <v>0.45138888888888878</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.4513888888888888</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
       <c r="A53" s="1">
         <v>53</v>
       </c>
       <c r="B53">
-        <v>0.56944444444444442</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.5694444444444444</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
       <c r="A54" s="1">
         <v>54</v>
       </c>
       <c r="B54">
-        <v>0.63194444444444442</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.6319444444444444</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
       <c r="A55" s="1">
         <v>55</v>
       </c>
@@ -843,31 +812,31 @@
         <v>1.395833333333333</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2">
       <c r="A56" s="1">
         <v>56</v>
       </c>
       <c r="B56">
-        <v>0.88194444444444442</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.8819444444444444</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
       <c r="A57" s="1">
         <v>57</v>
       </c>
       <c r="B57">
-        <v>0.95138888888888895</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.951388888888889</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
       <c r="A58" s="1">
         <v>58</v>
       </c>
       <c r="B58">
-        <v>1.1736111111111109</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1.173611111111111</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
       <c r="A59" s="1">
         <v>59</v>
       </c>
@@ -875,15 +844,15 @@
         <v>1.1875</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2">
       <c r="A60" s="1">
         <v>60</v>
       </c>
       <c r="B60">
-        <v>2.5694444444444442</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2.569444444444444</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
       <c r="A61" s="1">
         <v>61</v>
       </c>
@@ -891,7 +860,7 @@
         <v>1.6875</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2">
       <c r="A62" s="1">
         <v>62</v>
       </c>
@@ -899,7 +868,7 @@
         <v>1.145833333333333</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2">
       <c r="A63" s="1">
         <v>63</v>
       </c>
@@ -907,7 +876,7 @@
         <v>1.055555555555556</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2">
       <c r="A64" s="1">
         <v>64</v>
       </c>
@@ -915,15 +884,15 @@
         <v>1.166666666666667</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2">
       <c r="A65" s="1">
         <v>65</v>
       </c>
       <c r="B65">
-        <v>1.8472222222222221</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1.847222222222222</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
       <c r="A66" s="1">
         <v>66</v>
       </c>
@@ -931,23 +900,23 @@
         <v>1.3125</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2">
       <c r="A67" s="1">
         <v>67</v>
       </c>
       <c r="B67">
-        <v>1.1527777777777779</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1.152777777777778</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
       <c r="A68" s="1">
         <v>68</v>
       </c>
       <c r="B68">
-        <v>0.96527777777777779</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.9652777777777778</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
       <c r="A69" s="1">
         <v>69</v>
       </c>
@@ -955,15 +924,15 @@
         <v>1.083333333333333</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2">
       <c r="A70" s="1">
         <v>70</v>
       </c>
       <c r="B70">
-        <v>2.6736111111111112</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2.673611111111111</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
       <c r="A71" s="1">
         <v>71</v>
       </c>
@@ -971,39 +940,39 @@
         <v>1.180555555555556</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2">
       <c r="A72" s="1">
         <v>72</v>
       </c>
       <c r="B72">
-        <v>1.1180555555555549</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1.118055555555555</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
       <c r="A73" s="1">
         <v>73</v>
       </c>
       <c r="B73">
-        <v>1.0277777777777779</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1.027777777777778</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
       <c r="A74" s="1">
         <v>74</v>
       </c>
       <c r="B74">
-        <v>1.0277777777777779</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1.027777777777778</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
       <c r="A75" s="1">
         <v>75</v>
       </c>
       <c r="B75">
-        <v>1.7777777777777779</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1.777777777777778</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
       <c r="A76" s="1">
         <v>76</v>
       </c>
@@ -1011,15 +980,15 @@
         <v>0.9375</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2">
       <c r="A77" s="1">
         <v>77</v>
       </c>
       <c r="B77">
-        <v>1.1597222222222221</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1.159722222222222</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
       <c r="A78" s="1">
         <v>78</v>
       </c>
@@ -1027,47 +996,47 @@
         <v>1.104166666666667</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2">
       <c r="A79" s="1">
         <v>79</v>
       </c>
       <c r="B79">
-        <v>0.93055555555555547</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.9305555555555555</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
       <c r="A80" s="1">
         <v>80</v>
       </c>
       <c r="B80">
-        <v>2.6597222222222219</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2.659722222222222</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
       <c r="A81" s="1">
         <v>81</v>
       </c>
       <c r="B81">
-        <v>1.4236111111111109</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1.423611111111111</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
       <c r="A82" s="1">
         <v>82</v>
       </c>
       <c r="B82">
-        <v>1.0902777777777779</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1.090277777777778</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
       <c r="A83" s="1">
         <v>83</v>
       </c>
       <c r="B83">
-        <v>0.94444444444444442</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.9444444444444444</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
       <c r="A84" s="1">
         <v>84</v>
       </c>
@@ -1075,47 +1044,47 @@
         <v>1.0625</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2">
       <c r="A85" s="1">
         <v>85</v>
       </c>
       <c r="B85">
-        <v>1.7986111111111109</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1.798611111111111</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
       <c r="A86" s="1">
         <v>86</v>
       </c>
       <c r="B86">
-        <v>0.79861111111111105</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.798611111111111</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
       <c r="A87" s="1">
         <v>87</v>
       </c>
       <c r="B87">
-        <v>0.64583333333333337</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.6458333333333334</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
       <c r="A88" s="1">
         <v>88</v>
       </c>
       <c r="B88">
-        <v>0.73611111111111105</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.736111111111111</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
       <c r="A89" s="1">
         <v>89</v>
       </c>
       <c r="B89">
-        <v>0.65972222222222221</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.6597222222222222</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
       <c r="A90" s="1">
         <v>90</v>
       </c>
@@ -1123,90 +1092,84 @@
         <v>2.104166666666667</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2">
       <c r="A91" s="1">
         <v>91</v>
       </c>
       <c r="B91">
-        <v>0.71527777777777779</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.7152777777777778</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
       <c r="A92" s="1">
         <v>92</v>
       </c>
       <c r="B92">
-        <v>0.66666666666666674</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.6666666666666667</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
       <c r="A93" s="1">
         <v>93</v>
       </c>
       <c r="B93">
-        <v>0.76388888888888884</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.7638888888888888</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
       <c r="A94" s="1">
         <v>94</v>
       </c>
       <c r="B94">
-        <v>0.56944444444444442</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.5694444444444444</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
       <c r="A95" s="1">
         <v>95</v>
       </c>
       <c r="B95">
-        <v>1.7986111111111109</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1.798611111111111</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
       <c r="A96" s="1">
         <v>96</v>
       </c>
       <c r="B96">
-        <v>0.61805555555555558</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.6180555555555556</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
       <c r="A97" s="1">
         <v>97</v>
       </c>
       <c r="B97">
-        <v>0.51388888888888895</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.513888888888889</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
       <c r="A98" s="1">
         <v>98</v>
       </c>
       <c r="B98">
-        <v>0.59027777777777779</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.5902777777777778</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
       <c r="A99" s="1">
         <v>99</v>
       </c>
       <c r="B99">
-        <v>0.39583333333333343</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.3958333333333334</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
       <c r="A100" s="1">
         <v>100</v>
       </c>
       <c r="B100">
-        <v>5.5763888888888893</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B101">
-        <f>SUM(B1:B100)</f>
-        <v>100</v>
+        <v>5.576388888888889</v>
       </c>
     </row>
   </sheetData>

</xml_diff>